<commit_message>
v4 of manuscript with updated Mcap DGE analysis
</commit_message>
<xml_diff>
--- a/Sample_Info/samples_Mcapitata.annotations.xlsx
+++ b/Sample_Info/samples_Mcapitata.annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinchille/Documents/Rutgers/DBlab/repos.nosync/Genotype_dominates_transcriptomic_response_Pacu/Sample_Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B335BF-84E7-1E4B-8602-E5BD566C2DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5FD019-6CC7-FA47-B473-F0FC7F07D58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="460" windowWidth="14200" windowHeight="15860" xr2:uid="{099C7B7F-E81E-734B-B4DA-7DFE0E082013}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{099C7B7F-E81E-734B-B4DA-7DFE0E082013}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="164">
   <si>
     <t>Sample</t>
   </si>
@@ -71,45 +71,21 @@
     <t>Reef.35.36</t>
   </si>
   <si>
-    <t>TP4</t>
-  </si>
-  <si>
     <t>ATAC</t>
   </si>
   <si>
-    <t>Amb</t>
-  </si>
-  <si>
     <t>Reef.42.43</t>
   </si>
   <si>
-    <t>TP6</t>
-  </si>
-  <si>
     <t>HIMB</t>
   </si>
   <si>
-    <t>TP2</t>
-  </si>
-  <si>
     <t>Reef.11.13</t>
   </si>
   <si>
-    <t>TP7</t>
-  </si>
-  <si>
-    <t>TP3</t>
-  </si>
-  <si>
     <t>Reef.18</t>
   </si>
   <si>
-    <t>TP5</t>
-  </si>
-  <si>
-    <t>TP1</t>
-  </si>
-  <si>
     <t>Lilipuna.Fringe</t>
   </si>
   <si>
@@ -119,15 +95,9 @@
     <t>High</t>
   </si>
   <si>
-    <t>TP8</t>
-  </si>
-  <si>
     <t>HTAC</t>
   </si>
   <si>
-    <t>Hot</t>
-  </si>
-  <si>
     <t>HTHC</t>
   </si>
   <si>
@@ -524,14 +494,50 @@
     <t>Mcapitata_HTHC_TP12_2190</t>
   </si>
   <si>
-    <t>Mcapitata_HTAC_TP1_2153</t>
+    <t>Mcapitata_HTAC_TP4_2153</t>
+  </si>
+  <si>
+    <t>Ambient</t>
+  </si>
+  <si>
+    <t>0_hour</t>
+  </si>
+  <si>
+    <t>6_hour</t>
+  </si>
+  <si>
+    <t>12_hour</t>
+  </si>
+  <si>
+    <t>30_hour</t>
+  </si>
+  <si>
+    <t>1_week</t>
+  </si>
+  <si>
+    <t>2_week</t>
+  </si>
+  <si>
+    <t>4_week</t>
+  </si>
+  <si>
+    <t>6_week</t>
+  </si>
+  <si>
+    <t>8_week</t>
+  </si>
+  <si>
+    <t>12_week</t>
+  </si>
+  <si>
+    <t>16_week</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -543,13 +549,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -575,10 +574,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,6 +592,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,13 +897,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED66AA7-DA61-6E44-8CCE-7760E7442EF0}">
   <dimension ref="A1:H133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -932,24 +934,24 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2">
@@ -958,25 +960,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H3">
         <v>6</v>
@@ -984,25 +986,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -1010,25 +1012,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1036,25 +1038,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
+        <v>154</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
       </c>
       <c r="H6">
         <v>8</v>
@@ -1062,25 +1064,25 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -1088,24 +1090,24 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" t="s">
         <v>9</v>
       </c>
       <c r="H8">
@@ -1114,25 +1116,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H9">
         <v>6</v>
@@ -1140,25 +1142,25 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" t="s">
         <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H10">
         <v>8</v>
@@ -1166,25 +1168,25 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>156</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1192,25 +1194,25 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" t="s">
         <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H12">
         <v>6</v>
@@ -1218,25 +1220,25 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G13" t="s">
         <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H13">
         <v>8</v>
@@ -1244,25 +1246,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14" t="s">
         <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -1270,25 +1272,25 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" t="s">
         <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -1296,25 +1298,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>20</v>
+        <v>157</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
       </c>
       <c r="H16">
         <v>8</v>
@@ -1322,25 +1324,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>23</v>
+        <v>158</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1348,24 +1350,24 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" t="s">
         <v>9</v>
       </c>
       <c r="H18">
@@ -1374,24 +1376,24 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" t="s">
         <v>9</v>
       </c>
       <c r="H19">
@@ -1400,24 +1402,24 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" t="s">
         <v>9</v>
       </c>
       <c r="H20">
@@ -1426,24 +1428,24 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G21" t="s">
         <v>9</v>
       </c>
       <c r="H21">
@@ -1452,25 +1454,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22" t="s">
         <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H22">
         <v>8</v>
@@ -1478,25 +1480,25 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" t="s">
         <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1504,24 +1506,24 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" t="s">
         <v>9</v>
       </c>
       <c r="H24">
@@ -1530,24 +1532,24 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" t="s">
         <v>9</v>
       </c>
       <c r="H25">
@@ -1556,24 +1558,24 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" t="s">
         <v>9</v>
       </c>
       <c r="H26">
@@ -1582,25 +1584,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>17</v>
+        <v>161</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
       </c>
       <c r="H27">
         <v>8</v>
@@ -1608,25 +1610,25 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" t="s">
         <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H28">
         <v>6</v>
@@ -1634,24 +1636,24 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" t="s">
         <v>9</v>
       </c>
       <c r="H29">
@@ -1660,25 +1662,25 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" t="s">
         <v>12</v>
-      </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H30">
         <v>8</v>
@@ -1686,25 +1688,25 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F31" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" t="s">
         <v>14</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="H31">
         <v>6</v>
@@ -1712,25 +1714,25 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
       </c>
       <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" t="s">
         <v>11</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -1738,24 +1740,24 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" t="s">
         <v>9</v>
       </c>
       <c r="H33">
@@ -1764,25 +1766,25 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>20</v>
+        <v>163</v>
+      </c>
+      <c r="G34" t="s">
+        <v>14</v>
       </c>
       <c r="H34">
         <v>8</v>
@@ -1790,25 +1792,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E35" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>17</v>
+        <v>153</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
       </c>
       <c r="H35">
         <v>3</v>
@@ -1816,25 +1818,25 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>17</v>
+        <v>153</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
       </c>
       <c r="H36">
         <v>12</v>
@@ -1842,24 +1844,24 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" t="s">
         <v>9</v>
       </c>
       <c r="H37">
@@ -1868,25 +1870,25 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E38" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F38" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" t="s">
         <v>14</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="H38">
         <v>3</v>
@@ -1894,25 +1896,25 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>13</v>
+        <v>154</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
       </c>
       <c r="H39">
         <v>11</v>
@@ -1920,25 +1922,25 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" t="s">
         <v>12</v>
-      </c>
-      <c r="E40" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H40">
         <v>12</v>
@@ -1946,24 +1948,24 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G41" t="s">
         <v>9</v>
       </c>
       <c r="H41">
@@ -1972,25 +1974,25 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F42" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" t="s">
         <v>14</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="H42">
         <v>12</v>
@@ -1998,25 +2000,25 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E43" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>13</v>
+        <v>155</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
       </c>
       <c r="H43">
         <v>11</v>
@@ -2024,25 +2026,25 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F44" t="s">
-        <v>21</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>13</v>
+        <v>156</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
       </c>
       <c r="H44">
         <v>3</v>
@@ -2050,25 +2052,25 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E45" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F45" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>17</v>
+        <v>156</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
       </c>
       <c r="H45">
         <v>11</v>
@@ -2076,24 +2078,24 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E46" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" t="s">
         <v>9</v>
       </c>
       <c r="H46">
@@ -2102,25 +2104,25 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F47" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>17</v>
+        <v>157</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
       </c>
       <c r="H47">
         <v>3</v>
@@ -2128,24 +2130,24 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E48" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G48" t="s">
         <v>9</v>
       </c>
       <c r="H48">
@@ -2154,25 +2156,25 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E49" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F49" t="s">
-        <v>21</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>20</v>
+        <v>157</v>
+      </c>
+      <c r="G49" t="s">
+        <v>14</v>
       </c>
       <c r="H49">
         <v>12</v>
@@ -2180,25 +2182,25 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E50" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>13</v>
+        <v>158</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
       </c>
       <c r="H50">
         <v>3</v>
@@ -2206,25 +2208,25 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D51" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" t="s">
+        <v>158</v>
+      </c>
+      <c r="G51" t="s">
         <v>12</v>
-      </c>
-      <c r="E51" t="s">
-        <v>25</v>
-      </c>
-      <c r="F51" t="s">
-        <v>21</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H51">
         <v>11</v>
@@ -2232,25 +2234,25 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D52" t="s">
+        <v>152</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" t="s">
+        <v>158</v>
+      </c>
+      <c r="G52" t="s">
         <v>12</v>
-      </c>
-      <c r="E52" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" t="s">
-        <v>16</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H52">
         <v>12</v>
@@ -2258,24 +2260,24 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F53" t="s">
-        <v>16</v>
-      </c>
-      <c r="G53" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G53" t="s">
         <v>9</v>
       </c>
       <c r="H53">
@@ -2284,25 +2286,25 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E54" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F54" t="s">
-        <v>18</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>13</v>
+        <v>159</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
       </c>
       <c r="H54">
         <v>11</v>
@@ -2310,25 +2312,25 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E55" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F55" t="s">
-        <v>14</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>13</v>
+        <v>159</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
       </c>
       <c r="H55">
         <v>12</v>
@@ -2336,25 +2338,25 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E56" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F56" t="s">
-        <v>22</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>13</v>
+        <v>160</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
       </c>
       <c r="H56">
         <v>3</v>
@@ -2362,25 +2364,25 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" t="s">
         <v>12</v>
-      </c>
-      <c r="E57" t="s">
-        <v>25</v>
-      </c>
-      <c r="F57" t="s">
-        <v>21</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H57">
         <v>11</v>
@@ -2388,25 +2390,25 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E58" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>17</v>
+        <v>160</v>
+      </c>
+      <c r="G58" t="s">
+        <v>13</v>
       </c>
       <c r="H58">
         <v>12</v>
@@ -2414,25 +2416,25 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E59" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F59" t="s">
-        <v>21</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>17</v>
+        <v>161</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
       </c>
       <c r="H59">
         <v>3</v>
@@ -2440,25 +2442,25 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E60" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F60" t="s">
+        <v>161</v>
+      </c>
+      <c r="G60" t="s">
         <v>14</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="H60">
         <v>12</v>
@@ -2466,24 +2468,24 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E61" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F61" t="s">
-        <v>16</v>
-      </c>
-      <c r="G61" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G61" t="s">
         <v>9</v>
       </c>
       <c r="H61">
@@ -2492,24 +2494,24 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E62" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>16</v>
-      </c>
-      <c r="G62" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G62" t="s">
         <v>9</v>
       </c>
       <c r="H62">
@@ -2518,24 +2520,24 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E63" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F63" t="s">
-        <v>16</v>
-      </c>
-      <c r="G63" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G63" t="s">
         <v>9</v>
       </c>
       <c r="H63">
@@ -2544,25 +2546,25 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E64" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F64" t="s">
-        <v>26</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>13</v>
+        <v>162</v>
+      </c>
+      <c r="G64" t="s">
+        <v>11</v>
       </c>
       <c r="H64">
         <v>12</v>
@@ -2570,25 +2572,25 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D65" t="s">
+        <v>152</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>163</v>
+      </c>
+      <c r="G65" t="s">
         <v>12</v>
-      </c>
-      <c r="E65" t="s">
-        <v>25</v>
-      </c>
-      <c r="F65" t="s">
-        <v>14</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H65">
         <v>3</v>
@@ -2596,25 +2598,25 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E66" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F66" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>13</v>
+        <v>163</v>
+      </c>
+      <c r="G66" t="s">
+        <v>11</v>
       </c>
       <c r="H66">
         <v>11</v>
@@ -2622,25 +2624,25 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="E67" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>20</v>
+        <v>163</v>
+      </c>
+      <c r="G67" t="s">
+        <v>14</v>
       </c>
       <c r="H67">
         <v>12</v>
@@ -2648,25 +2650,25 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D68" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E68" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F68" t="s">
-        <v>21</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>23</v>
+        <v>153</v>
+      </c>
+      <c r="G68" t="s">
+        <v>15</v>
       </c>
       <c r="H68">
         <v>7</v>
@@ -2674,25 +2676,25 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E69" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F69" t="s">
-        <v>10</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>13</v>
+        <v>153</v>
+      </c>
+      <c r="G69" t="s">
+        <v>11</v>
       </c>
       <c r="H69">
         <v>9</v>
@@ -2700,24 +2702,24 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D70" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E70" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F70" t="s">
-        <v>21</v>
-      </c>
-      <c r="G70" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G70" t="s">
         <v>9</v>
       </c>
       <c r="H70">
@@ -2726,25 +2728,25 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D71" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E71" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F71" t="s">
-        <v>19</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>13</v>
+        <v>154</v>
+      </c>
+      <c r="G71" t="s">
+        <v>11</v>
       </c>
       <c r="H71">
         <v>7</v>
@@ -2752,25 +2754,25 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B72" t="s">
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D72" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E72" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F72" t="s">
-        <v>14</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>13</v>
+        <v>154</v>
+      </c>
+      <c r="G72" t="s">
+        <v>11</v>
       </c>
       <c r="H72">
         <v>9</v>
@@ -2778,24 +2780,24 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F73" t="s">
-        <v>16</v>
-      </c>
-      <c r="G73" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G73" t="s">
         <v>9</v>
       </c>
       <c r="H73">
@@ -2804,24 +2806,24 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E74" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F74" t="s">
-        <v>26</v>
-      </c>
-      <c r="G74" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G74" t="s">
         <v>9</v>
       </c>
       <c r="H74">
@@ -2830,25 +2832,25 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D75" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E75" t="s">
+        <v>152</v>
+      </c>
+      <c r="F75" t="s">
+        <v>155</v>
+      </c>
+      <c r="G75" t="s">
         <v>12</v>
-      </c>
-      <c r="F75" t="s">
-        <v>22</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H75">
         <v>9</v>
@@ -2856,25 +2858,25 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D76" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E76" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F76" t="s">
-        <v>22</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>20</v>
+        <v>155</v>
+      </c>
+      <c r="G76" t="s">
+        <v>14</v>
       </c>
       <c r="H76">
         <v>4</v>
@@ -2882,25 +2884,25 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D77" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E77" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F77" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>17</v>
+        <v>156</v>
+      </c>
+      <c r="G77" t="s">
+        <v>13</v>
       </c>
       <c r="H77">
         <v>4</v>
@@ -2908,25 +2910,25 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B78" t="s">
         <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D78" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E78" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F78" t="s">
-        <v>16</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>23</v>
+        <v>156</v>
+      </c>
+      <c r="G78" t="s">
+        <v>15</v>
       </c>
       <c r="H78">
         <v>7</v>
@@ -2934,25 +2936,25 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D79" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E79" t="s">
+        <v>152</v>
+      </c>
+      <c r="F79" t="s">
+        <v>156</v>
+      </c>
+      <c r="G79" t="s">
         <v>12</v>
-      </c>
-      <c r="F79" t="s">
-        <v>19</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H79">
         <v>9</v>
@@ -2960,24 +2962,24 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D80" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E80" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F80" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G80" t="s">
         <v>9</v>
       </c>
       <c r="H80">
@@ -2986,25 +2988,25 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E81" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F81" t="s">
-        <v>10</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>20</v>
+        <v>157</v>
+      </c>
+      <c r="G81" t="s">
+        <v>14</v>
       </c>
       <c r="H81">
         <v>4</v>
@@ -3012,24 +3014,24 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E82" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F82" t="s">
-        <v>19</v>
-      </c>
-      <c r="G82" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G82" t="s">
         <v>9</v>
       </c>
       <c r="H82">
@@ -3038,25 +3040,25 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D83" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E83" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F83" t="s">
-        <v>14</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>17</v>
+        <v>158</v>
+      </c>
+      <c r="G83" t="s">
+        <v>13</v>
       </c>
       <c r="H83">
         <v>4</v>
@@ -3064,25 +3066,25 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D84" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E84" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F84" t="s">
-        <v>16</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>13</v>
+        <v>158</v>
+      </c>
+      <c r="G84" t="s">
+        <v>11</v>
       </c>
       <c r="H84">
         <v>7</v>
@@ -3090,24 +3092,24 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D85" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E85" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F85" t="s">
-        <v>21</v>
-      </c>
-      <c r="G85" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G85" t="s">
         <v>9</v>
       </c>
       <c r="H85">
@@ -3116,25 +3118,25 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D86" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E86" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F86" t="s">
-        <v>22</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>13</v>
+        <v>159</v>
+      </c>
+      <c r="G86" t="s">
+        <v>11</v>
       </c>
       <c r="H86">
         <v>4</v>
@@ -3142,25 +3144,25 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D87" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E87" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F87" t="s">
-        <v>26</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>20</v>
+        <v>159</v>
+      </c>
+      <c r="G87" t="s">
+        <v>14</v>
       </c>
       <c r="H87">
         <v>7</v>
@@ -3168,25 +3170,25 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D88" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E88" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F88" t="s">
-        <v>10</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>20</v>
+        <v>159</v>
+      </c>
+      <c r="G88" t="s">
+        <v>14</v>
       </c>
       <c r="H88">
         <v>9</v>
@@ -3194,25 +3196,25 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D89" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E89" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F89" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>23</v>
+        <v>160</v>
+      </c>
+      <c r="G89" t="s">
+        <v>15</v>
       </c>
       <c r="H89">
         <v>4</v>
@@ -3220,25 +3222,25 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D90" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E90" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F90" t="s">
-        <v>21</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>17</v>
+        <v>160</v>
+      </c>
+      <c r="G90" t="s">
+        <v>13</v>
       </c>
       <c r="H90">
         <v>7</v>
@@ -3246,25 +3248,25 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D91" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E91" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F91" t="s">
-        <v>10</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>20</v>
+        <v>160</v>
+      </c>
+      <c r="G91" t="s">
+        <v>14</v>
       </c>
       <c r="H91">
         <v>9</v>
@@ -3272,25 +3274,25 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D92" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E92" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F92" t="s">
-        <v>10</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>23</v>
+        <v>161</v>
+      </c>
+      <c r="G92" t="s">
+        <v>15</v>
       </c>
       <c r="H92">
         <v>4</v>
@@ -3298,25 +3300,25 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B93" t="s">
         <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D93" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E93" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F93" t="s">
-        <v>18</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>17</v>
+        <v>161</v>
+      </c>
+      <c r="G93" t="s">
+        <v>13</v>
       </c>
       <c r="H93">
         <v>7</v>
@@ -3324,25 +3326,25 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B94" t="s">
         <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D94" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E94" t="s">
+        <v>152</v>
+      </c>
+      <c r="F94" t="s">
+        <v>161</v>
+      </c>
+      <c r="G94" t="s">
         <v>12</v>
-      </c>
-      <c r="F94" t="s">
-        <v>19</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H94">
         <v>9</v>
@@ -3350,25 +3352,25 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B95" t="s">
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D95" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E95" t="s">
+        <v>152</v>
+      </c>
+      <c r="F95" t="s">
+        <v>162</v>
+      </c>
+      <c r="G95" t="s">
         <v>12</v>
-      </c>
-      <c r="F95" t="s">
-        <v>21</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H95">
         <v>4</v>
@@ -3376,25 +3378,25 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B96" t="s">
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D96" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E96" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F96" t="s">
-        <v>22</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>17</v>
+        <v>162</v>
+      </c>
+      <c r="G96" t="s">
+        <v>13</v>
       </c>
       <c r="H96">
         <v>9</v>
@@ -3402,25 +3404,25 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B97" t="s">
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D97" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E97" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F97" t="s">
+        <v>162</v>
+      </c>
+      <c r="G97" t="s">
         <v>14</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="H97">
         <v>7</v>
@@ -3428,25 +3430,25 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D98" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E98" t="s">
+        <v>152</v>
+      </c>
+      <c r="F98" t="s">
+        <v>163</v>
+      </c>
+      <c r="G98" t="s">
         <v>12</v>
-      </c>
-      <c r="F98" t="s">
-        <v>22</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H98">
         <v>7</v>
@@ -3454,25 +3456,25 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E99" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F99" t="s">
-        <v>22</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>20</v>
+        <v>163</v>
+      </c>
+      <c r="G99" t="s">
+        <v>14</v>
       </c>
       <c r="H99">
         <v>4</v>
@@ -3480,25 +3482,25 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D100" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E100" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F100" t="s">
-        <v>18</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>13</v>
+        <v>163</v>
+      </c>
+      <c r="G100" t="s">
+        <v>11</v>
       </c>
       <c r="H100">
         <v>9</v>
@@ -3506,25 +3508,25 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B101" t="s">
         <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D101" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E101" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F101" t="s">
-        <v>19</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>15</v>
+        <v>153</v>
+      </c>
+      <c r="G101" t="s">
+        <v>12</v>
       </c>
       <c r="H101">
         <v>2</v>
@@ -3532,24 +3534,24 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D102" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E102" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F102" t="s">
-        <v>26</v>
-      </c>
-      <c r="G102" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G102" t="s">
         <v>9</v>
       </c>
       <c r="H102">
@@ -3558,25 +3560,25 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D103" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E103" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F103" t="s">
-        <v>16</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>15</v>
+        <v>153</v>
+      </c>
+      <c r="G103" t="s">
+        <v>12</v>
       </c>
       <c r="H103">
         <v>10</v>
@@ -3584,25 +3586,25 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D104" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E104" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F104" t="s">
-        <v>26</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>15</v>
+        <v>154</v>
+      </c>
+      <c r="G104" t="s">
+        <v>12</v>
       </c>
       <c r="H104">
         <v>2</v>
@@ -3610,25 +3612,25 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B105" t="s">
         <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D105" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E105" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F105" t="s">
-        <v>21</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>15</v>
+        <v>154</v>
+      </c>
+      <c r="G105" t="s">
+        <v>12</v>
       </c>
       <c r="H105">
         <v>5</v>
@@ -3636,25 +3638,25 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B106" t="s">
         <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D106" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E106" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F106" t="s">
-        <v>16</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>20</v>
+        <v>154</v>
+      </c>
+      <c r="G106" t="s">
+        <v>14</v>
       </c>
       <c r="H106">
         <v>10</v>
@@ -3662,25 +3664,25 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D107" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E107" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F107" t="s">
-        <v>10</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>13</v>
+        <v>155</v>
+      </c>
+      <c r="G107" t="s">
+        <v>11</v>
       </c>
       <c r="H107">
         <v>2</v>
@@ -3688,25 +3690,25 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D108" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E108" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F108" t="s">
-        <v>21</v>
-      </c>
-      <c r="G108" s="2" t="s">
-        <v>17</v>
+        <v>155</v>
+      </c>
+      <c r="G108" t="s">
+        <v>13</v>
       </c>
       <c r="H108">
         <v>5</v>
@@ -3714,25 +3716,25 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B109" t="s">
         <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D109" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E109" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F109" t="s">
-        <v>18</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>13</v>
+        <v>155</v>
+      </c>
+      <c r="G109" t="s">
+        <v>11</v>
       </c>
       <c r="H109">
         <v>10</v>
@@ -3740,25 +3742,25 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B110" t="s">
         <v>8</v>
       </c>
       <c r="C110" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D110" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E110" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F110" t="s">
-        <v>22</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>20</v>
+        <v>156</v>
+      </c>
+      <c r="G110" t="s">
+        <v>14</v>
       </c>
       <c r="H110">
         <v>2</v>
@@ -3766,25 +3768,25 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B111" t="s">
         <v>8</v>
       </c>
       <c r="C111" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D111" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E111" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F111" t="s">
-        <v>16</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>23</v>
+        <v>156</v>
+      </c>
+      <c r="G111" t="s">
+        <v>15</v>
       </c>
       <c r="H111">
         <v>5</v>
@@ -3792,25 +3794,25 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
       </c>
       <c r="C112" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D112" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E112" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F112" t="s">
-        <v>18</v>
-      </c>
-      <c r="G112" s="2" t="s">
-        <v>17</v>
+        <v>156</v>
+      </c>
+      <c r="G112" t="s">
+        <v>13</v>
       </c>
       <c r="H112">
         <v>10</v>
@@ -3818,24 +3820,24 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B113" t="s">
         <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D113" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E113" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F113" t="s">
-        <v>18</v>
-      </c>
-      <c r="G113" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G113" t="s">
         <v>9</v>
       </c>
       <c r="H113">
@@ -3844,24 +3846,24 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B114" t="s">
         <v>8</v>
       </c>
       <c r="C114" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D114" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E114" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F114" t="s">
-        <v>19</v>
-      </c>
-      <c r="G114" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G114" t="s">
         <v>9</v>
       </c>
       <c r="H114">
@@ -3870,25 +3872,25 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B115" t="s">
         <v>8</v>
       </c>
       <c r="C115" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D115" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E115" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F115" t="s">
-        <v>10</v>
-      </c>
-      <c r="G115" s="2" t="s">
-        <v>17</v>
+        <v>157</v>
+      </c>
+      <c r="G115" t="s">
+        <v>13</v>
       </c>
       <c r="H115">
         <v>10</v>
@@ -3896,25 +3898,25 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B116" t="s">
         <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D116" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E116" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F116" t="s">
-        <v>16</v>
-      </c>
-      <c r="G116" s="2" t="s">
-        <v>13</v>
+        <v>158</v>
+      </c>
+      <c r="G116" t="s">
+        <v>11</v>
       </c>
       <c r="H116">
         <v>2</v>
@@ -3922,25 +3924,25 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B117" t="s">
         <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D117" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E117" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F117" t="s">
-        <v>26</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>13</v>
+        <v>158</v>
+      </c>
+      <c r="G117" t="s">
+        <v>11</v>
       </c>
       <c r="H117">
         <v>5</v>
@@ -3948,25 +3950,25 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B118" t="s">
         <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D118" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E118" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F118" t="s">
-        <v>21</v>
-      </c>
-      <c r="G118" s="2" t="s">
-        <v>20</v>
+        <v>158</v>
+      </c>
+      <c r="G118" t="s">
+        <v>14</v>
       </c>
       <c r="H118">
         <v>10</v>
@@ -3974,25 +3976,25 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B119" t="s">
         <v>8</v>
       </c>
       <c r="C119" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D119" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E119" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F119" t="s">
-        <v>22</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>17</v>
+        <v>159</v>
+      </c>
+      <c r="G119" t="s">
+        <v>13</v>
       </c>
       <c r="H119">
         <v>2</v>
@@ -4000,25 +4002,25 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B120" t="s">
         <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D120" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E120" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F120" t="s">
-        <v>10</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>13</v>
+        <v>159</v>
+      </c>
+      <c r="G120" t="s">
+        <v>11</v>
       </c>
       <c r="H120">
         <v>5</v>
@@ -4026,25 +4028,25 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B121" t="s">
         <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D121" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E121" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F121" t="s">
-        <v>16</v>
-      </c>
-      <c r="G121" s="2" t="s">
-        <v>15</v>
+        <v>159</v>
+      </c>
+      <c r="G121" t="s">
+        <v>12</v>
       </c>
       <c r="H121">
         <v>10</v>
@@ -4052,25 +4054,25 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
       </c>
       <c r="C122" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D122" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E122" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F122" t="s">
-        <v>16</v>
-      </c>
-      <c r="G122" s="2" t="s">
-        <v>17</v>
+        <v>160</v>
+      </c>
+      <c r="G122" t="s">
+        <v>13</v>
       </c>
       <c r="H122">
         <v>2</v>
@@ -4078,25 +4080,25 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B123" t="s">
         <v>8</v>
       </c>
       <c r="C123" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D123" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E123" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F123" t="s">
-        <v>19</v>
-      </c>
-      <c r="G123" s="2" t="s">
-        <v>17</v>
+        <v>160</v>
+      </c>
+      <c r="G123" t="s">
+        <v>13</v>
       </c>
       <c r="H123">
         <v>5</v>
@@ -4104,25 +4106,25 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D124" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E124" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F124" t="s">
-        <v>10</v>
-      </c>
-      <c r="G124" s="2" t="s">
-        <v>23</v>
+        <v>160</v>
+      </c>
+      <c r="G124" t="s">
+        <v>15</v>
       </c>
       <c r="H124">
         <v>10</v>
@@ -4130,25 +4132,25 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D125" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E125" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F125" t="s">
-        <v>14</v>
-      </c>
-      <c r="G125" s="2" t="s">
-        <v>17</v>
+        <v>161</v>
+      </c>
+      <c r="G125" t="s">
+        <v>13</v>
       </c>
       <c r="H125">
         <v>2</v>
@@ -4156,25 +4158,25 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B126" t="s">
         <v>8</v>
       </c>
       <c r="C126" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D126" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E126" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F126" t="s">
-        <v>19</v>
-      </c>
-      <c r="G126" s="2" t="s">
-        <v>17</v>
+        <v>161</v>
+      </c>
+      <c r="G126" t="s">
+        <v>13</v>
       </c>
       <c r="H126">
         <v>5</v>
@@ -4182,25 +4184,25 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B127" t="s">
         <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D127" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E127" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F127" t="s">
-        <v>22</v>
-      </c>
-      <c r="G127" s="2" t="s">
-        <v>17</v>
+        <v>161</v>
+      </c>
+      <c r="G127" t="s">
+        <v>13</v>
       </c>
       <c r="H127">
         <v>10</v>
@@ -4208,25 +4210,25 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B128" t="s">
         <v>8</v>
       </c>
       <c r="C128" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D128" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E128" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F128" t="s">
-        <v>10</v>
-      </c>
-      <c r="G128" s="2" t="s">
-        <v>23</v>
+        <v>162</v>
+      </c>
+      <c r="G128" t="s">
+        <v>15</v>
       </c>
       <c r="H128">
         <v>2</v>
@@ -4234,25 +4236,25 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B129" t="s">
         <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D129" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E129" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F129" t="s">
-        <v>22</v>
-      </c>
-      <c r="G129" s="2" t="s">
-        <v>15</v>
+        <v>162</v>
+      </c>
+      <c r="G129" t="s">
+        <v>12</v>
       </c>
       <c r="H129">
         <v>5</v>
@@ -4260,25 +4262,25 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B130" t="s">
         <v>8</v>
       </c>
       <c r="C130" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D130" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E130" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F130" t="s">
-        <v>21</v>
-      </c>
-      <c r="G130" s="2" t="s">
-        <v>20</v>
+        <v>162</v>
+      </c>
+      <c r="G130" t="s">
+        <v>14</v>
       </c>
       <c r="H130">
         <v>10</v>
@@ -4286,25 +4288,25 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B131" t="s">
         <v>8</v>
       </c>
       <c r="C131" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D131" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E131" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F131" t="s">
-        <v>19</v>
-      </c>
-      <c r="G131" s="2" t="s">
-        <v>15</v>
+        <v>163</v>
+      </c>
+      <c r="G131" t="s">
+        <v>12</v>
       </c>
       <c r="H131">
         <v>2</v>
@@ -4312,25 +4314,25 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B132" t="s">
         <v>8</v>
       </c>
       <c r="C132" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D132" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E132" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F132" t="s">
-        <v>16</v>
-      </c>
-      <c r="G132" s="2" t="s">
-        <v>15</v>
+        <v>163</v>
+      </c>
+      <c r="G132" t="s">
+        <v>12</v>
       </c>
       <c r="H132">
         <v>5</v>
@@ -4338,32 +4340,31 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B133" t="s">
         <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D133" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E133" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F133" t="s">
-        <v>10</v>
-      </c>
-      <c r="G133" s="2" t="s">
-        <v>13</v>
+        <v>163</v>
+      </c>
+      <c r="G133" t="s">
+        <v>11</v>
       </c>
       <c r="H133">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H133" xr:uid="{1ED66AA7-DA61-6E44-8CCE-7760E7442EF0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>